<commit_message>
Initial commit -  new model
</commit_message>
<xml_diff>
--- a/data/WorkTypes.xlsx
+++ b/data/WorkTypes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\forlogssystems\work_utilization_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60EDC2EB-C527-4748-AA93-C6DF2822CF08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47138283-731A-4CE0-969A-FF9C7E835599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>213 Pick3PL_Astro</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>206 Replenishment</t>
+  </si>
+  <si>
+    <t>202 Goods receive G</t>
   </si>
 </sst>
 </file>
@@ -378,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,54 +398,86 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>0</v>
-      </c>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>